<commit_message>
clean cn data, still need to confirm sample IDs
</commit_message>
<xml_diff>
--- a/data/cn/raw/pp_spb_cn_2021.03.12.xlsx
+++ b/data/cn/raw/pp_spb_cn_2021.03.12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/risa/Git/pitch_pine_spb/data/cn/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55568B30-2D14-458A-9027-8DB709C936D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B2DB61-9ABD-0F4A-A855-158334A88129}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{CEE89D7D-ADB2-48F5-A45D-F75A6CFF0913}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24240" windowHeight="13140" xr2:uid="{CEE89D7D-ADB2-48F5-A45D-F75A6CFF0913}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1083,12 +1083,15 @@
   <dimension ref="A1:AM116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD58"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="F2" t="s">
         <v>5</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1421,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1769,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1885,7 +1888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -2001,7 +2004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2117,7 +2120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2233,7 +2236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2349,7 +2352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -2465,7 +2468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2581,7 +2584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -2697,7 +2700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -2813,7 +2816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -2929,7 +2932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -3045,7 +3048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -3161,7 +3164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -3393,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -3509,7 +3512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -3625,7 +3628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3741,7 +3744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -3857,7 +3860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -3973,7 +3976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>70</v>
       </c>
@@ -4089,7 +4092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -4205,7 +4208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -4321,7 +4324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -4437,7 +4440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -4553,7 +4556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>80</v>
       </c>
@@ -4669,7 +4672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -4785,7 +4788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -4901,7 +4904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -5017,7 +5020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>88</v>
       </c>
@@ -5133,7 +5136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -5249,7 +5252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>92</v>
       </c>
@@ -5365,7 +5368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -5481,7 +5484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>96</v>
       </c>
@@ -5597,7 +5600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>98</v>
       </c>
@@ -5713,7 +5716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>100</v>
       </c>
@@ -5829,7 +5832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>101</v>
       </c>
@@ -5945,7 +5948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>102</v>
       </c>
@@ -6061,7 +6064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -6177,7 +6180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -6293,7 +6296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -6409,7 +6412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -6525,7 +6528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>107</v>
       </c>
@@ -6641,7 +6644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -6757,7 +6760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>109</v>
       </c>
@@ -6873,7 +6876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>110</v>
       </c>
@@ -6989,7 +6992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -7105,7 +7108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -7221,7 +7224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -7337,7 +7340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>117</v>
       </c>
@@ -7453,7 +7456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -7569,7 +7572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -7685,7 +7688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>123</v>
       </c>
@@ -7801,7 +7804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>125</v>
       </c>
@@ -7917,7 +7920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -8033,7 +8036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>129</v>
       </c>
@@ -8149,7 +8152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -8265,7 +8268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>132</v>
       </c>
@@ -8381,7 +8384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>134</v>
       </c>
@@ -8497,7 +8500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>136</v>
       </c>
@@ -8613,7 +8616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>138</v>
       </c>
@@ -8729,7 +8732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>140</v>
       </c>
@@ -8845,7 +8848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>142</v>
       </c>
@@ -8961,7 +8964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>144</v>
       </c>
@@ -9077,7 +9080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>146</v>
       </c>
@@ -9193,7 +9196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>148</v>
       </c>
@@ -9309,7 +9312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>150</v>
       </c>
@@ -9425,7 +9428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>152</v>
       </c>
@@ -9541,7 +9544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>154</v>
       </c>
@@ -9657,7 +9660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>156</v>
       </c>
@@ -9773,7 +9776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>158</v>
       </c>
@@ -9889,7 +9892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>160</v>
       </c>
@@ -10005,7 +10008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>162</v>
       </c>
@@ -10121,7 +10124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>164</v>
       </c>
@@ -10237,7 +10240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>166</v>
       </c>
@@ -10353,7 +10356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>168</v>
       </c>
@@ -10469,7 +10472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>170</v>
       </c>
@@ -10585,7 +10588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>172</v>
       </c>
@@ -10701,7 +10704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>174</v>
       </c>
@@ -10817,7 +10820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>176</v>
       </c>
@@ -10933,7 +10936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>178</v>
       </c>
@@ -11049,7 +11052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>180</v>
       </c>
@@ -11165,7 +11168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>182</v>
       </c>
@@ -11281,7 +11284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>184</v>
       </c>
@@ -11397,7 +11400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>186</v>
       </c>
@@ -11513,7 +11516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>188</v>
       </c>
@@ -11629,7 +11632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>190</v>
       </c>
@@ -11745,7 +11748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>192</v>
       </c>
@@ -11861,7 +11864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>194</v>
       </c>
@@ -11977,7 +11980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>196</v>
       </c>
@@ -12093,7 +12096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>198</v>
       </c>
@@ -12209,7 +12212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>200</v>
       </c>
@@ -12325,7 +12328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>202</v>
       </c>
@@ -12441,7 +12444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>204</v>
       </c>
@@ -12557,7 +12560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>206</v>
       </c>
@@ -12673,7 +12676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>208</v>
       </c>
@@ -12789,7 +12792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>210</v>
       </c>
@@ -12905,7 +12908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>211</v>
       </c>
@@ -13021,7 +13024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>213</v>
       </c>
@@ -13137,7 +13140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>215</v>
       </c>
@@ -13253,7 +13256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>216</v>
       </c>
@@ -13369,7 +13372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>218</v>
       </c>
@@ -13485,7 +13488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>219</v>
       </c>
@@ -13601,7 +13604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>221</v>
       </c>
@@ -13717,7 +13720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>222</v>
       </c>
@@ -13833,7 +13836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>224</v>
       </c>
@@ -13949,7 +13952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>225</v>
       </c>
@@ -14065,7 +14068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>227</v>
       </c>
@@ -14181,7 +14184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>229</v>
       </c>
@@ -14297,7 +14300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>230</v>
       </c>
@@ -14413,7 +14416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>231</v>
       </c>

</xml_diff>